<commit_message>
Fix Flat Type data not printing
</commit_message>
<xml_diff>
--- a/src/main/resources/data/ProjectList.xlsx
+++ b/src/main/resources/data/ProjectList.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10402"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jordanchoi/IdeaProjects/SC2002 FCSD Group 2 HDB BTO/src/main/resources/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/2179e81e572d34a2/Documents/GitHub/sc2002_hdb_fcsd_group2/src/main/resources/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C693CC14-B1F6-2A47-9E5F-038FD14A9902}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="5" documentId="13_ncr:1_{C693CC14-B1F6-2A47-9E5F-038FD14A9902}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A9A18629-8A53-42A0-A17E-ECC08327B6A4}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="19940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="29055" yWindow="2205" windowWidth="27075" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -165,6 +165,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -433,27 +437,27 @@
   <dimension ref="A1:M5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="99" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.33203125" customWidth="1"/>
-    <col min="2" max="2" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.1640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.1640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.1640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.1640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20.33203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="19.5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="7.6640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.28515625" customWidth="1"/>
+    <col min="2" max="2" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.7109375" customWidth="1"/>
+    <col min="4" max="4" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14" customWidth="1"/>
+    <col min="7" max="7" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="28.140625" customWidth="1"/>
+    <col min="9" max="9" width="31.85546875" customWidth="1"/>
+    <col min="10" max="10" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.7109375" customWidth="1"/>
+    <col min="13" max="13" width="16.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -494,7 +498,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>19</v>
       </c>
@@ -535,7 +539,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -576,7 +580,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -617,7 +621,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>21</v>
       </c>

</xml_diff>

<commit_message>
Add Approve/Reject Officer Project Request
</commit_message>
<xml_diff>
--- a/src/main/resources/data/ProjectList.xlsx
+++ b/src/main/resources/data/ProjectList.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/2179e81e572d34a2/Documents/GitHub/sc2002_hdb_fcsd_group2/src/main/resources/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="33" documentId="13_ncr:1_{C693CC14-B1F6-2A47-9E5F-038FD14A9902}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{943851E2-DBD2-4830-9CFE-B8E1B624C3AD}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="109_{6891E820-AE69-40B0-B404-C2B94F5127E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1335" yWindow="2625" windowWidth="28335" windowHeight="12225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="3255" windowWidth="28335" windowHeight="12225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -111,13 +111,13 @@
     <t>Emily</t>
   </si>
   <si>
-    <t>Daniel, Emily, David</t>
-  </si>
-  <si>
     <t>Visibilty</t>
   </si>
   <si>
     <t>Project Id</t>
+  </si>
+  <si>
+    <t>Daniel, Emily</t>
   </si>
 </sst>
 </file>
@@ -153,10 +153,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -172,10 +171,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -444,7 +439,7 @@
   <dimension ref="A1:O5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="99" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="O10" sqref="O10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -469,7 +464,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -508,14 +503,14 @@
         <v>14</v>
       </c>
       <c r="O1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B2">
         <v>1</v>
       </c>
       <c r="C2" t="s">
@@ -562,7 +557,7 @@
       <c r="A3" t="s">
         <v>20</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B3">
         <v>2</v>
       </c>
       <c r="C3" t="s">
@@ -609,7 +604,7 @@
       <c r="A4" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B4">
         <v>3</v>
       </c>
       <c r="C4" t="s">
@@ -656,7 +651,7 @@
       <c r="A5" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="2">
+      <c r="B5">
         <v>4</v>
       </c>
       <c r="C5" t="s">
@@ -693,7 +688,7 @@
         <v>10</v>
       </c>
       <c r="N5" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="O5" t="b">
         <v>1</v>

</xml_diff>